<commit_message>
fix: fix problem in the index
</commit_message>
<xml_diff>
--- a/media/requisition_1.xlsx
+++ b/media/requisition_1.xlsx
@@ -550,7 +550,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>RAD123456</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>OP12345</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H6" s="3" t="n"/>
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="C8" s="6" t="n">
-        <v>-692739</v>
+        <v>45427</v>
       </c>
       <c r="D8" s="7" t="n"/>
       <c r="E8" s="7" t="n"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="C9" s="8" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D9" s="7" t="n"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>1234567890</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D10" s="7" t="n"/>
@@ -622,7 +622,7 @@
       </c>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>Cargo X</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D11" s="7" t="n"/>
@@ -638,7 +638,7 @@
       </c>
       <c r="C12" s="8" t="inlineStr">
         <is>
-          <t>Dependencia Y</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D12" s="7" t="n"/>
@@ -654,7 +654,7 @@
       </c>
       <c r="C13" s="8" t="inlineStr">
         <is>
-          <t>CENCO123</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D13" s="7" t="n"/>
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="C14" s="8" t="n">
-        <v>100000</v>
+        <v>1</v>
       </c>
       <c r="D14" s="7" t="n"/>
       <c r="E14" s="7" t="n"/>
@@ -708,7 +708,7 @@
       <c r="A18" s="3" t="n"/>
       <c r="B18" s="7" t="inlineStr">
         <is>
-          <t>Descripción de la requisición</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C18" s="7" t="n"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="G30" s="12" t="inlineStr">
         <is>
-          <t>0987654321</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H30" s="3" t="n"/>
@@ -857,12 +857,12 @@
     <row r="34">
       <c r="B34" s="13" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E34" s="13" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H34" s="3" t="n"/>
@@ -886,12 +886,12 @@
     <row r="37">
       <c r="B37" s="13" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E37" s="13" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H37" s="3" t="n"/>

</xml_diff>